<commit_message>
added for loop for multi files
</commit_message>
<xml_diff>
--- a/2018-11-02__RBKT1.xlsx
+++ b/2018-11-02__RBKT1.xlsx
@@ -4013,12 +4013,12 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4028,6 +4028,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF008000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4049,7 +4055,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>